<commit_message>
update fix template and apps
</commit_message>
<xml_diff>
--- a/template/matakuliah_template.xlsx
+++ b/template/matakuliah_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Mata Kuliah" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>No</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>(SI, S2, S3)</t>
+  </si>
+  <si>
+    <t>ID_SMS</t>
   </si>
 </sst>
 </file>
@@ -616,98 +619,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" customWidth="1"/>
-    <col min="17" max="17" width="22.28515625" customWidth="1"/>
-    <col min="18" max="18" width="25.42578125" customWidth="1"/>
-    <col min="19" max="19" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.88671875" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="19" max="19" width="25.44140625" customWidth="1"/>
+    <col min="20" max="20" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -721,8 +727,9 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="6"/>
+      <c r="R2" s="4"/>
       <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -734,17 +741,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -755,7 +762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -766,7 +773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -777,7 +784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>4</v>
       </c>
@@ -788,7 +795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>5</v>
       </c>
@@ -799,7 +806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -810,7 +817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -821,7 +828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -832,7 +839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -843,7 +850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -854,7 +861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -865,7 +872,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -876,7 +883,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -887,7 +894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -898,7 +905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -909,7 +916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>16</v>
       </c>

</xml_diff>